<commit_message>
Excel Update and enum driven
</commit_message>
<xml_diff>
--- a/src/test/resources/InstanceDetails.xlsx
+++ b/src/test/resources/InstanceDetails.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>Instance Name</t>
   </si>
@@ -87,46 +87,76 @@
     <t>password</t>
   </si>
   <si>
-    <t>company_name</t>
-  </si>
-  <si>
-    <t>auth_type</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
-    <t>mailbox_email</t>
-  </si>
-  <si>
     <t>OAuth</t>
   </si>
   <si>
     <t>vendor</t>
   </si>
   <si>
-    <t>sx_inbound</t>
-  </si>
-  <si>
-    <t>application_Id</t>
-  </si>
-  <si>
-    <t>tenant_id</t>
-  </si>
-  <si>
-    <t>secret_key</t>
-  </si>
-  <si>
-    <t>display_name</t>
-  </si>
-  <si>
-    <t>object_id</t>
-  </si>
-  <si>
     <t>TestingProd</t>
   </si>
   <si>
     <t>supporttest@bigfixsm.io</t>
+  </si>
+  <si>
+    <t>companyName</t>
+  </si>
+  <si>
+    <t>mailboxEmail</t>
+  </si>
+  <si>
+    <t>authType</t>
+  </si>
+  <si>
+    <t>sxInbound</t>
+  </si>
+  <si>
+    <t>applicationId</t>
+  </si>
+  <si>
+    <t>tenantId</t>
+  </si>
+  <si>
+    <t>secretKey</t>
+  </si>
+  <si>
+    <t>displayName</t>
+  </si>
+  <si>
+    <t>objectId</t>
+  </si>
+  <si>
+    <t>offeringName</t>
+  </si>
+  <si>
+    <t>whitelistedDomains</t>
+  </si>
+  <si>
+    <t>alwaysProcessException</t>
+  </si>
+  <si>
+    <t>neverProcessException</t>
+  </si>
+  <si>
+    <t>defaultImpact</t>
+  </si>
+  <si>
+    <t>defaultUrgency</t>
+  </si>
+  <si>
+    <t>userVerificationType</t>
+  </si>
+  <si>
+    <t>guestUserEmail</t>
+  </si>
+  <si>
+    <t>guestUserName</t>
+  </si>
+  <si>
+    <t>actionStatus</t>
   </si>
 </sst>
 </file>
@@ -460,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -477,9 +507,19 @@
     <col min="10" max="10" width="29.90625" customWidth="1"/>
     <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="19.54296875" customWidth="1"/>
+    <col min="18" max="18" width="26.453125" customWidth="1"/>
+    <col min="19" max="19" width="23.6328125" customWidth="1"/>
+    <col min="20" max="20" width="16.453125" customWidth="1"/>
+    <col min="21" max="21" width="15.54296875" customWidth="1"/>
+    <col min="22" max="22" width="19.81640625" customWidth="1"/>
+    <col min="23" max="23" width="18.453125" customWidth="1"/>
+    <col min="24" max="24" width="17.08984375" customWidth="1"/>
+    <col min="25" max="25" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,40 +533,70 @@
         <v>21</v>
       </c>
       <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O1" t="s">
-        <v>33</v>
+        <v>35</v>
+      </c>
+      <c r="P1" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -549,7 +619,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>8</v>
@@ -561,7 +631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" s="1" customFormat="1" ht="145" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -584,7 +654,7 @@
         <v>9</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>8</v>
@@ -602,9 +672,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="145" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" s="1" customFormat="1" ht="145" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
@@ -619,13 +689,13 @@
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>8</v>

</xml_diff>